<commit_message>
Adding in jupyter code for Muon Lifetime Lab
</commit_message>
<xml_diff>
--- a/Muon/Muon.xlsx
+++ b/Muon/Muon.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\OneDrive\Documents\University\Eng\Third Year\ENPH353\Muon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a82bfad6b286b01a/Documents/University/Eng/Third Year/ENPH353/Muon/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="6510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4290" windowHeight="5595"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="alex2colinmuonlabovernight" localSheetId="0">Sheet1!$K$33:$K$2090</definedName>
+    <definedName name="alex2colinmuonlabovernight" localSheetId="0">Sheet1!$K$33:$K$2076</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>Value</t>
   </si>
@@ -134,33 +134,6 @@
     <t>R mean</t>
   </si>
   <si>
-    <t>$ROI:</t>
-  </si>
-  <si>
-    <t>$PRESETS:</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>$ENER_FIT:</t>
-  </si>
-  <si>
-    <t>-0.097933 0.001067</t>
-  </si>
-  <si>
-    <t>$MCA_CAL:</t>
-  </si>
-  <si>
-    <t>-9.793330E-002 1.067114E-003 0.000000E+000</t>
-  </si>
-  <si>
-    <t>$SHAPE_CAL:</t>
-  </si>
-  <si>
-    <t>0.000000E+000 0.000000E+000 0.000000E+000</t>
-  </si>
-  <si>
     <t>Fit Results</t>
   </si>
   <si>
@@ -189,6 +162,51 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Overnight:</t>
+  </si>
+  <si>
+    <t>Bin fit</t>
+  </si>
+  <si>
+    <t>Bin std</t>
+  </si>
+  <si>
+    <t>Fit slope</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>us/bin</t>
+  </si>
+  <si>
+    <t>er</t>
+  </si>
+  <si>
+    <t>Physical Representation</t>
+  </si>
+  <si>
+    <t>Nb</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Muon Lifetime</t>
+  </si>
+  <si>
+    <t>Number of particles</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
+  <si>
+    <t>Constant back ground</t>
   </si>
 </sst>
 </file>
@@ -233,12 +251,12 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14773,10 +14791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q2090"/>
+  <dimension ref="A2:X2076"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14785,28 +14803,32 @@
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="11" max="11" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="21" max="21" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -14837,8 +14859,38 @@
       <c r="L3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R3" t="s">
+        <v>48</v>
+      </c>
+      <c r="T3" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" t="s">
+        <v>49</v>
+      </c>
+      <c r="V3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -14872,8 +14924,38 @@
       <c r="L4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>101</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="T4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U4" t="s">
+        <v>53</v>
+      </c>
+      <c r="V4">
+        <v>157</v>
+      </c>
+      <c r="W4">
+        <v>2</v>
+      </c>
+      <c r="X4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -14909,8 +14991,29 @@
       <c r="L5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>166</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" t="s">
+        <v>52</v>
+      </c>
+      <c r="V5">
+        <v>2.754</v>
+      </c>
+      <c r="W5">
+        <v>0.1</v>
+      </c>
+      <c r="X5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -14945,8 +15048,29 @@
       <c r="L6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>278</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U6" t="s">
+        <v>55</v>
+      </c>
+      <c r="V6">
+        <v>13.3</v>
+      </c>
+      <c r="W6">
+        <v>0.2</v>
+      </c>
+      <c r="X6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -14980,8 +15104,14 @@
       <c r="L7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>359</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -15016,8 +15146,14 @@
       <c r="L8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>441</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F9">
         <v>6</v>
       </c>
@@ -15039,8 +15175,14 @@
       <c r="L9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>524</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F10">
         <v>7</v>
       </c>
@@ -15062,8 +15204,14 @@
       <c r="L10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>624</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F11">
         <v>8</v>
       </c>
@@ -15085,8 +15233,14 @@
       <c r="L11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>721</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F12">
         <v>9</v>
       </c>
@@ -15108,8 +15262,14 @@
       <c r="L12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>812</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F13">
         <v>10</v>
       </c>
@@ -15131,8 +15291,19 @@
       <c r="L13">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>903</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -15140,7 +15311,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -15970,6 +16141,17 @@
         <v>33.93325156280256</v>
       </c>
     </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>42</v>
+      </c>
+      <c r="K32" t="s">
+        <v>41</v>
+      </c>
+      <c r="L32" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K33">
         <v>129</v>
@@ -15980,7 +16162,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="K34">
         <v>111</v>
@@ -15991,16 +16173,16 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="K35">
         <v>138</v>
@@ -16010,11 +16192,11 @@
       </c>
     </row>
     <row r="36" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>44</v>
+      <c r="A36" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C36">
         <v>166</v>
@@ -16031,10 +16213,10 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C37">
         <v>116</v>
@@ -16050,11 +16232,11 @@
       </c>
     </row>
     <row r="38" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>49</v>
+      <c r="A38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C38">
         <v>13.5</v>
@@ -32371,76 +32553,6 @@
       </c>
       <c r="L2076">
         <v>2044</v>
-      </c>
-    </row>
-    <row r="2077" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K2077" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2078" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K2078">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2079" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K2079" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2080" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K2080" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2081" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K2081">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2082" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K2082">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2083" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K2083" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2084" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K2084" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2085" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K2085" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2086" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K2086">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2087" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K2087" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2088" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K2088" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2089" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K2089">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2090" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K2090" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding CE calibration and updated excel file
</commit_message>
<xml_diff>
--- a/Muon/Muon.xlsx
+++ b/Muon/Muon.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
   <si>
     <t>Value</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>V er</t>
-  </si>
-  <si>
-    <t>Bin er</t>
   </si>
   <si>
     <t xml:space="preserve">Threshold [V ] </t>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>Constant back ground</t>
+  </si>
+  <si>
+    <t>Bin Estimate</t>
   </si>
 </sst>
 </file>
@@ -14494,6 +14494,52 @@
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="alex2colinmuonlabovernight" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="F3:M13" totalsRowShown="0">
+  <autoFilter ref="F3:M13">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Trial"/>
+    <tableColumn id="2" name="Period [us]"/>
+    <tableColumn id="3" name="Period er"/>
+    <tableColumn id="4" name="Voltage pk-pk [V]"/>
+    <tableColumn id="5" name="V er"/>
+    <tableColumn id="6" name="Bin Estimate"/>
+    <tableColumn id="7" name="Bin fit"/>
+    <tableColumn id="8" name="Bin std"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="S3:W6" totalsRowShown="0">
+  <autoFilter ref="S3:W6">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Symbol"/>
+    <tableColumn id="2" name="Physical Representation"/>
+    <tableColumn id="3" name="Value"/>
+    <tableColumn id="4" name="Error"/>
+    <tableColumn id="5" name="Unit"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -14791,10 +14837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:X2076"/>
+  <dimension ref="A2:W2076"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14803,15 +14849,17 @@
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="19" max="19" width="9.7109375" customWidth="1"/>
+    <col min="20" max="20" width="24.42578125" customWidth="1"/>
     <col min="21" max="21" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -14828,7 +14876,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -14854,43 +14902,40 @@
         <v>19</v>
       </c>
       <c r="K3" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="L3" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="M3" t="s">
         <v>43</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>44</v>
       </c>
       <c r="P3" t="s">
         <v>45</v>
       </c>
       <c r="Q3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S3" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" t="s">
         <v>48</v>
       </c>
-      <c r="T3" t="s">
-        <v>32</v>
-      </c>
       <c r="U3" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="V3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="W3" t="s">
-        <v>34</v>
-      </c>
-      <c r="X3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -14922,40 +14967,37 @@
         <v>101</v>
       </c>
       <c r="L4">
+        <v>101</v>
+      </c>
+      <c r="M4">
         <v>1</v>
       </c>
-      <c r="M4">
-        <v>101</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="P4">
+      <c r="O4">
         <v>2.2200000000000001E-2</v>
       </c>
-      <c r="Q4" t="s">
-        <v>47</v>
-      </c>
-      <c r="R4">
+      <c r="P4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4">
         <v>2.9999999999999997E-4</v>
       </c>
+      <c r="S4" t="s">
+        <v>35</v>
+      </c>
       <c r="T4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U4" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="U4">
+        <v>157</v>
       </c>
       <c r="V4">
-        <v>157</v>
-      </c>
-      <c r="W4">
         <v>2</v>
       </c>
-      <c r="X4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -14989,31 +15031,28 @@
         <v>165</v>
       </c>
       <c r="L5">
+        <v>166</v>
+      </c>
+      <c r="M5">
         <v>1</v>
       </c>
-      <c r="M5">
-        <v>166</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U5" t="s">
-        <v>52</v>
+      <c r="S5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" t="s">
+        <v>51</v>
+      </c>
+      <c r="U5">
+        <v>2.754</v>
       </c>
       <c r="V5">
-        <v>2.754</v>
-      </c>
-      <c r="W5">
         <v>0.1</v>
       </c>
-      <c r="X5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -15046,31 +15085,28 @@
         <v>267</v>
       </c>
       <c r="L6">
+        <v>278</v>
+      </c>
+      <c r="M6">
         <v>1</v>
       </c>
-      <c r="M6">
-        <v>278</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="T6" s="2" t="s">
+      <c r="S6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T6" t="s">
+        <v>54</v>
+      </c>
+      <c r="U6">
+        <v>13.3</v>
+      </c>
+      <c r="V6">
+        <v>0.2</v>
+      </c>
+      <c r="W6" t="s">
         <v>50</v>
       </c>
-      <c r="U6" t="s">
-        <v>55</v>
-      </c>
-      <c r="V6">
-        <v>13.3</v>
-      </c>
-      <c r="W6">
-        <v>0.2</v>
-      </c>
-      <c r="X6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -15102,16 +15138,13 @@
         <v>359</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>359</v>
       </c>
       <c r="M7">
-        <v>359</v>
-      </c>
-      <c r="N7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -15144,16 +15177,13 @@
         <v>441</v>
       </c>
       <c r="L8">
+        <v>441</v>
+      </c>
+      <c r="M8">
         <v>1</v>
       </c>
-      <c r="M8">
-        <v>441</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F9">
         <v>6</v>
       </c>
@@ -15173,16 +15203,13 @@
         <v>524</v>
       </c>
       <c r="L9">
+        <v>524</v>
+      </c>
+      <c r="M9">
         <v>1</v>
       </c>
-      <c r="M9">
-        <v>524</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F10">
         <v>7</v>
       </c>
@@ -15202,16 +15229,13 @@
         <v>623</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>624</v>
       </c>
       <c r="M10">
-        <v>624</v>
-      </c>
-      <c r="N10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F11">
         <v>8</v>
       </c>
@@ -15231,16 +15255,13 @@
         <v>720</v>
       </c>
       <c r="L11">
+        <v>721</v>
+      </c>
+      <c r="M11">
         <v>1</v>
       </c>
-      <c r="M11">
-        <v>721</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F12">
         <v>9</v>
       </c>
@@ -15260,16 +15281,13 @@
         <v>811</v>
       </c>
       <c r="L12">
+        <v>812</v>
+      </c>
+      <c r="M12">
         <v>1</v>
       </c>
-      <c r="M12">
-        <v>812</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F13">
         <v>10</v>
       </c>
@@ -15289,76 +15307,73 @@
         <v>902</v>
       </c>
       <c r="L13">
+        <v>903</v>
+      </c>
+      <c r="M13">
         <v>1</v>
       </c>
-      <c r="M13">
-        <v>903</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="N14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" t="s">
         <v>28</v>
       </c>
-      <c r="J15" t="s">
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="J16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s">
+      <c r="L16" t="s">
         <v>22</v>
       </c>
-      <c r="C16" t="s">
+      <c r="M16" t="s">
         <v>23</v>
       </c>
-      <c r="D16" t="s">
+      <c r="N16" t="s">
         <v>24</v>
       </c>
-      <c r="E16" t="s">
+      <c r="O16" t="s">
         <v>25</v>
       </c>
-      <c r="F16" t="s">
+      <c r="P16" t="s">
         <v>26</v>
       </c>
-      <c r="G16" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J16" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16" t="s">
-        <v>24</v>
-      </c>
-      <c r="N16" t="s">
-        <v>25</v>
-      </c>
-      <c r="O16" t="s">
-        <v>26</v>
-      </c>
-      <c r="P16" t="s">
-        <v>27</v>
-      </c>
       <c r="Q16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -16143,10 +16158,10 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L32" t="s">
         <v>12</v>
@@ -16162,7 +16177,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K34">
         <v>111</v>
@@ -16173,16 +16188,16 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K35">
         <v>138</v>
@@ -16193,10 +16208,10 @@
     </row>
     <row r="36" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
         <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>36</v>
       </c>
       <c r="C36">
         <v>166</v>
@@ -16213,10 +16228,10 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C37">
         <v>116</v>
@@ -16233,10 +16248,10 @@
     </row>
     <row r="38" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C38">
         <v>13.5</v>
@@ -32563,5 +32578,9 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="2">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>